<commit_message>
update some variable codes
</commit_message>
<xml_diff>
--- a/data-viz/inputs/report_outline.xlsx
+++ b/data-viz/inputs/report_outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhabiby\Documents\GitHub\eu-gpp-report\data-viz\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A6486F-776D-4B3A-9DD2-F46ADDF8F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D485EA8-CDDE-4065-8B75-8F1C4356B464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{6CDB5189-70D4-4DC8-80AA-E85435BE4D53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6CDB5189-70D4-4DC8-80AA-E85435BE4D53}"/>
   </bookViews>
   <sheets>
     <sheet name="outline" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3367" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="1099">
   <si>
     <t>ID</t>
   </si>
@@ -3263,6 +3263,90 @@
   </si>
   <si>
     <t>Freedom</t>
+  </si>
+  <si>
+    <t>COR_judges</t>
+  </si>
+  <si>
+    <t>Corruption</t>
+  </si>
+  <si>
+    <t>COR_prosecutors</t>
+  </si>
+  <si>
+    <t>COR_pda</t>
+  </si>
+  <si>
+    <t>COR_police</t>
+  </si>
+  <si>
+    <t>JSE_rightsaware</t>
+  </si>
+  <si>
+    <t>JSE_access2info</t>
+  </si>
+  <si>
+    <t>JSE_access2assis</t>
+  </si>
+  <si>
+    <t>JSE_affordcosts</t>
+  </si>
+  <si>
+    <t>JSE_quickresol</t>
+  </si>
+  <si>
+    <t>JSE_fairoutcomes</t>
+  </si>
+  <si>
+    <t>JSE_equality</t>
+  </si>
+  <si>
+    <t>JSE_enforce</t>
+  </si>
+  <si>
+    <t>JSE_mediation</t>
+  </si>
+  <si>
+    <t>SEC_walking</t>
+  </si>
+  <si>
+    <t>SEC_home</t>
+  </si>
+  <si>
+    <t>SEC_street</t>
+  </si>
+  <si>
+    <t>SEC_children</t>
+  </si>
+  <si>
+    <t>SEC_women</t>
+  </si>
+  <si>
+    <t>SEC_lgbt</t>
+  </si>
+  <si>
+    <t>SEC_race</t>
+  </si>
+  <si>
+    <t>SEC_orgcrime</t>
+  </si>
+  <si>
+    <t>SEC_immigrant</t>
+  </si>
+  <si>
+    <t>LEP_safecom</t>
+  </si>
+  <si>
+    <t>LEP_safefam</t>
+  </si>
+  <si>
+    <t>LEP_policehelp</t>
+  </si>
+  <si>
+    <t>LEP_kindpol</t>
+  </si>
+  <si>
+    <t>LEP_lawacts</t>
   </si>
 </sst>
 </file>
@@ -3717,8 +3801,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3944,9 +4028,11 @@
         <v>4</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>1071</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>1072</v>
+      </c>
       <c r="H6" s="6" t="s">
         <v>23</v>
       </c>
@@ -3980,9 +4066,11 @@
         <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>1073</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>1072</v>
+      </c>
       <c r="H7" s="6" t="s">
         <v>23</v>
       </c>
@@ -4016,9 +4104,11 @@
         <v>13</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="6"/>
+        <v>1074</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1072</v>
+      </c>
       <c r="H8" s="6" t="s">
         <v>23</v>
       </c>
@@ -4052,9 +4142,11 @@
         <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="6"/>
+        <v>1075</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1072</v>
+      </c>
       <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
@@ -4088,7 +4180,7 @@
         <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>1076</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
@@ -4124,7 +4216,7 @@
         <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>45</v>
+        <v>1077</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
@@ -4160,7 +4252,7 @@
         <v>48</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>49</v>
+        <v>1078</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="s">
@@ -4196,7 +4288,7 @@
         <v>52</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>53</v>
+        <v>1079</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
@@ -4232,7 +4324,7 @@
         <v>56</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>57</v>
+        <v>1080</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
@@ -4268,7 +4360,7 @@
         <v>60</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>61</v>
+        <v>1081</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
@@ -4304,7 +4396,7 @@
         <v>64</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>65</v>
+        <v>1082</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
@@ -4340,7 +4432,7 @@
         <v>68</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>69</v>
+        <v>1083</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
@@ -4376,7 +4468,7 @@
         <v>72</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>73</v>
+        <v>1084</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -4844,9 +4936,8 @@
         <v>137</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="6"/>
+        <v>1085</v>
+      </c>
       <c r="H31" s="6" t="s">
         <v>139</v>
       </c>
@@ -4880,7 +4971,7 @@
         <v>142</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>143</v>
+        <v>1086</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6" t="s">
@@ -4916,7 +5007,7 @@
         <v>147</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>148</v>
+        <v>1087</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6" t="s">
@@ -4952,7 +5043,7 @@
         <v>151</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>152</v>
+        <v>1088</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6" t="s">
@@ -4988,7 +5079,7 @@
         <v>155</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>156</v>
+        <v>1089</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6" t="s">
@@ -5024,7 +5115,7 @@
         <v>159</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>160</v>
+        <v>1090</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6" t="s">
@@ -5060,7 +5151,7 @@
         <v>163</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>164</v>
+        <v>1091</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6" t="s">
@@ -5096,7 +5187,7 @@
         <v>167</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>168</v>
+        <v>1092</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6" t="s">
@@ -5132,7 +5223,7 @@
         <v>171</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>172</v>
+        <v>1093</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6" t="s">
@@ -5168,7 +5259,7 @@
         <v>176</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>177</v>
+        <v>1094</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6" t="s">
@@ -5204,7 +5295,7 @@
         <v>180</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>181</v>
+        <v>1095</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6" t="s">
@@ -5240,7 +5331,7 @@
         <v>184</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>185</v>
+        <v>1096</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6" t="s">
@@ -5276,7 +5367,7 @@
         <v>188</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>189</v>
+        <v>1097</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6" t="s">
@@ -5312,7 +5403,7 @@
         <v>192</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>193</v>
+        <v>1098</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6" t="s">
@@ -16226,6 +16317,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -16474,16 +16574,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E91D62-195B-4F39-8A40-C6DABBBF482D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCEE38A5-5C7B-472C-B7CC-7CE69A756247}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16500,12 +16599,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E91D62-195B-4F39-8A40-C6DABBBF482D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>